<commit_message>
Untitle 파일 삭제(단순 yfinance module 실행)
</commit_message>
<xml_diff>
--- a/241101.xlsx
+++ b/241101.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://skhynix-my.sharepoint.com/personal/2067609_skhynix_com/Documents/바탕 화면/jinhoon/developer/stockTrading/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="28" documentId="11_CA20A6B60FF76FFC05FC9890E2AC9AB40B117667" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8C6F09F5-DBF3-7149-BDC8-1B2F94680084}"/>
+  <xr:revisionPtr revIDLastSave="29" documentId="11_CA20A6B60FF76FFC05FC9890E2AC9AB40B117667" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B85D7407-7DE8-E54A-9954-DBF21054FE6D}"/>
   <bookViews>
-    <workbookView xWindow="39140" yWindow="20840" windowWidth="23040" windowHeight="20220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38400" yWindow="20740" windowWidth="23040" windowHeight="20220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -74,7 +74,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="176" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
-    <numFmt numFmtId="178" formatCode="0.0%"/>
+    <numFmt numFmtId="177" formatCode="0.0%"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -151,7 +151,7 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="백분율" xfId="1" builtinId="5"/>
@@ -1358,10 +1358,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L23"/>
+  <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17"/>
@@ -1950,9 +1950,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="3:12">
+    <row r="17" spans="5:12">
       <c r="E17" s="3">
-        <f t="shared" ref="E17:I17" si="0">+E14/E13-1</f>
+        <f t="shared" ref="E17:H17" si="0">+E14/E13-1</f>
         <v>-1.9627501638838529E-2</v>
       </c>
       <c r="F17" s="3">
@@ -1984,24 +1984,10 @@
         <v>3.289473684210531E-2</v>
       </c>
     </row>
-    <row r="21" spans="3:12">
-      <c r="C21">
-        <v>910</v>
-      </c>
+    <row r="21" spans="5:12">
       <c r="F21">
         <f>13*5</f>
         <v>65</v>
-      </c>
-    </row>
-    <row r="22" spans="3:12">
-      <c r="C22">
-        <v>673</v>
-      </c>
-    </row>
-    <row r="23" spans="3:12">
-      <c r="C23">
-        <f>+C21/C22-1</f>
-        <v>0.35215453194650825</v>
       </c>
     </row>
   </sheetData>

</xml_diff>